<commit_message>
updated to change to California dataset
</commit_message>
<xml_diff>
--- a/least_squares/error_stats.xlsx
+++ b/least_squares/error_stats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="3">
   <si>
     <t>Frac</t>
   </si>
@@ -42,7 +42,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -72,11 +72,17 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -100,6 +106,12 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -113,18 +125,18 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="true"/>
-    <col min="2" max="2" width="7.7109375" customWidth="true"/>
+    <col min="2" max="2" width="6.7109375" customWidth="true"/>
     <col min="3" max="3" width="6.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="27" t="s">
         <v>2</v>
       </c>
     </row>
@@ -133,10 +145,10 @@
         <v>0.20000000000000001</v>
       </c>
       <c r="B2">
-        <v>31.0566</v>
+        <v>0.36570000000000003</v>
       </c>
       <c r="C2">
-        <v>4.3067000000000002</v>
+        <v>0.0032000000000000002</v>
       </c>
     </row>
     <row r="3">
@@ -144,10 +156,10 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="B3">
-        <v>28.732700000000001</v>
+        <v>0.36509999999999998</v>
       </c>
       <c r="C3">
-        <v>3.1530999999999998</v>
+        <v>0.0041000000000000003</v>
       </c>
     </row>
     <row r="4">
@@ -155,10 +167,10 @@
         <v>0.40000000000000002</v>
       </c>
       <c r="B4">
-        <v>27.635899999999999</v>
+        <v>0.36480000000000001</v>
       </c>
       <c r="C4">
-        <v>3.2763</v>
+        <v>0.0045999999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -166,10 +178,10 @@
         <v>0.5</v>
       </c>
       <c r="B5">
-        <v>26.893699999999999</v>
+        <v>0.36580000000000001</v>
       </c>
       <c r="C5">
-        <v>3.6587000000000001</v>
+        <v>0.0068999999999999999</v>
       </c>
     </row>
     <row r="6">
@@ -177,10 +189,10 @@
         <v>0.59999999999999998</v>
       </c>
       <c r="B6">
-        <v>26.483799999999999</v>
+        <v>0.36499999999999999</v>
       </c>
       <c r="C6">
-        <v>4.4816000000000003</v>
+        <v>0.0079000000000000008</v>
       </c>
     </row>
     <row r="7">
@@ -188,10 +200,10 @@
         <v>0.69999999999999996</v>
       </c>
       <c r="B7">
-        <v>26.4817</v>
+        <v>0.36480000000000001</v>
       </c>
       <c r="C7">
-        <v>5.3681000000000001</v>
+        <v>0.0101</v>
       </c>
     </row>
     <row r="8">
@@ -199,10 +211,10 @@
         <v>0.80000000000000004</v>
       </c>
       <c r="B8">
-        <v>26.3992</v>
+        <v>0.36530000000000001</v>
       </c>
       <c r="C8">
-        <v>7.2484000000000002</v>
+        <v>0.0137</v>
       </c>
     </row>
     <row r="9">
@@ -210,10 +222,10 @@
         <v>0.90000000000000002</v>
       </c>
       <c r="B9">
-        <v>25.892099999999999</v>
+        <v>0.36230000000000001</v>
       </c>
       <c r="C9">
-        <v>10.867000000000001</v>
+        <v>0.020400000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed least squares and ridge regression, improving performance
</commit_message>
<xml_diff>
--- a/least_squares/error_stats.xlsx
+++ b/least_squares/error_stats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="3">
   <si>
     <t>Frac</t>
   </si>
@@ -42,7 +42,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -78,11 +78,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -112,6 +114,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -130,13 +134,13 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
     </row>
@@ -145,7 +149,7 @@
         <v>0.20000000000000001</v>
       </c>
       <c r="B2">
-        <v>0.36570000000000003</v>
+        <v>0.3659</v>
       </c>
       <c r="C2">
         <v>0.0032000000000000002</v>
@@ -156,7 +160,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="B3">
-        <v>0.36509999999999998</v>
+        <v>0.36530000000000001</v>
       </c>
       <c r="C3">
         <v>0.0041000000000000003</v>
@@ -170,7 +174,7 @@
         <v>0.36480000000000001</v>
       </c>
       <c r="C4">
-        <v>0.0045999999999999999</v>
+        <v>0.0051999999999999998</v>
       </c>
     </row>
     <row r="5">
@@ -178,10 +182,10 @@
         <v>0.5</v>
       </c>
       <c r="B5">
-        <v>0.36580000000000001</v>
+        <v>0.3649</v>
       </c>
       <c r="C5">
-        <v>0.0068999999999999999</v>
+        <v>0.0064999999999999997</v>
       </c>
     </row>
     <row r="6">
@@ -189,10 +193,10 @@
         <v>0.59999999999999998</v>
       </c>
       <c r="B6">
-        <v>0.36499999999999999</v>
+        <v>0.3649</v>
       </c>
       <c r="C6">
-        <v>0.0079000000000000008</v>
+        <v>0.0080000000000000002</v>
       </c>
     </row>
     <row r="7">
@@ -200,10 +204,10 @@
         <v>0.69999999999999996</v>
       </c>
       <c r="B7">
-        <v>0.36480000000000001</v>
+        <v>0.36470000000000002</v>
       </c>
       <c r="C7">
-        <v>0.0101</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="8">
@@ -211,10 +215,10 @@
         <v>0.80000000000000004</v>
       </c>
       <c r="B8">
-        <v>0.36530000000000001</v>
+        <v>0.3639</v>
       </c>
       <c r="C8">
-        <v>0.0137</v>
+        <v>0.012999999999999999</v>
       </c>
     </row>
     <row r="9">
@@ -222,10 +226,10 @@
         <v>0.90000000000000002</v>
       </c>
       <c r="B9">
-        <v>0.36230000000000001</v>
+        <v>0.36349999999999999</v>
       </c>
       <c r="C9">
-        <v>0.020400000000000001</v>
+        <v>0.019400000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>